<commit_message>
Atualizando dados do monitoramento
</commit_message>
<xml_diff>
--- a/Monitoramento (1).xlsx
+++ b/Monitoramento (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\higor\Documents\Lab.Tesla\CAD 3\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A26212-5D3F-46D6-AA84-2481F9DA3752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03451A11-2C41-4AF6-AF4D-E532448E07B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{F7F44B12-655A-4005-9057-50BCBCCFAD44}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{F7F44B12-655A-4005-9057-50BCBCCFAD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="21" r:id="rId1"/>
@@ -490,7 +490,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -660,7 +660,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
@@ -33597,8 +33596,8 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:R367"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33902,9 +33901,9 @@
       <c r="I6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="11">
-        <f>MEDIAN(B114:B144)</f>
-        <v>439</v>
+      <c r="J6" s="41">
+        <f>AVERAGE(B114:B144)</f>
+        <v>422.86774193548393</v>
       </c>
       <c r="K6" s="61">
         <f>SUM(B114:B144)/1000</f>
@@ -33954,9 +33953,9 @@
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="12">
-        <f>MEDIAN(B145:B174)</f>
-        <v>444.95</v>
+      <c r="J7" s="42">
+        <f>AVERAGE(B145:B174)</f>
+        <v>429.7766666666667</v>
       </c>
       <c r="K7" s="62">
         <f>SUM(B145:B174)/1000</f>
@@ -34006,9 +34005,9 @@
       <c r="I8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="11">
-        <f>MEDIAN(B175:B205)</f>
-        <v>450.8</v>
+      <c r="J8" s="41">
+        <f>AVERAGE(B175:B205)</f>
+        <v>434.77419354838707</v>
       </c>
       <c r="K8" s="61">
         <f>SUM(B175:B205)/1000</f>
@@ -34058,9 +34057,9 @@
       <c r="I9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="12">
-        <f>MEDIAN(B206:B236)</f>
-        <v>505.8</v>
+      <c r="J9" s="42">
+        <f>AVERAGE(B206:B236)</f>
+        <v>491.05161290322576</v>
       </c>
       <c r="K9" s="62">
         <f>SUM(B206:B237)/1000</f>
@@ -34110,9 +34109,9 @@
       <c r="I10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="11">
-        <f>MEDIAN(B237:B266)</f>
-        <v>593.79999999999995</v>
+      <c r="J10" s="41">
+        <f>AVERAGE(B237:B266)</f>
+        <v>556.69333333333338</v>
       </c>
       <c r="K10" s="61">
         <f>SUM(B237:B266)/1000</f>
@@ -34162,9 +34161,9 @@
       <c r="I11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="12">
-        <f>MEDIAN(B275:B305)</f>
-        <v>529.9</v>
+      <c r="J11" s="42">
+        <f>AVERAGE(B267:B297)</f>
+        <v>539.24193548387086</v>
       </c>
       <c r="K11" s="62">
         <f>SUM(B267:B297)/1000</f>
@@ -34172,15 +34171,15 @@
       </c>
       <c r="L11" s="20">
         <f>SUM(E275:E305)</f>
-        <v>87.540410958904133</v>
-      </c>
-      <c r="M11" s="28">
-        <f>J11/(R11*732*0.202)</f>
-        <v>0.63316228512152029</v>
+        <v>111.18698630136991</v>
+      </c>
+      <c r="M11" s="18">
+        <f>K11*1000/(R11*146*30)</f>
+        <v>0.67430256385433296</v>
       </c>
       <c r="N11" s="28">
         <f>MEDIAN(F276:F306)</f>
-        <v>0.12948059360730593</v>
+        <v>0.15139840182648401</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="15" t="s">
@@ -34214,22 +34213,25 @@
       <c r="I12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="11" t="e">
-        <f>MEDIAN(B307:B336)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K12" s="61"/>
+      <c r="J12" s="41">
+        <f>AVERAGE(B298:B327)</f>
+        <v>591.75666666666655</v>
+      </c>
+      <c r="K12" s="61">
+        <f>SUM(B298:B327)/1000</f>
+        <v>17.752699999999997</v>
+      </c>
       <c r="L12" s="16">
-        <f>SUM(E306:E336)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="18" t="e">
-        <f t="shared" ref="M12:M13" si="2">J12/(R12*732*0.202)</f>
-        <v>#NUM!</v>
+        <f>SUM(E298:E327)</f>
+        <v>121.59383561643834</v>
+      </c>
+      <c r="M12" s="18">
+        <f>K12*1000/(R12*146*30)</f>
+        <v>0.7575939913796782</v>
       </c>
       <c r="N12" s="18">
         <f>MEDIAN(F307:F336)</f>
-        <v>0</v>
+        <v>0.16141552511415524</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="13" t="s">
@@ -34273,7 +34275,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="28" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M13" si="2">J13/(R13*732*0.202)</f>
         <v>#NUM!</v>
       </c>
       <c r="N13" s="28">
@@ -34318,11 +34320,11 @@
       </c>
       <c r="K14" s="63">
         <f>SUM(K2:K13)</f>
-        <v>151.40290000000002</v>
+        <v>169.15560000000002</v>
       </c>
       <c r="L14" s="33">
         <f>SUM(L2:L13)</f>
-        <v>1009.5712328767123</v>
+        <v>1154.8116438356165</v>
       </c>
       <c r="M14" s="24" t="e">
         <f>J14/(R14*708*0.202)/12</f>
@@ -34330,7 +34332,7 @@
       </c>
       <c r="N14" s="26">
         <f>MEDIAN(N2:N13)</f>
-        <v>0.13237014840182648</v>
+        <v>0.14787385844748857</v>
       </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="29" t="s">
@@ -40570,7 +40572,7 @@
       <c r="A298" s="51">
         <v>45962.999305497688</v>
       </c>
-      <c r="B298" s="38">
+      <c r="B298">
         <v>650.4</v>
       </c>
       <c r="C298" s="3">
@@ -40592,7 +40594,9 @@
       <c r="A299" s="51">
         <v>45963.999305497688</v>
       </c>
-      <c r="B299" s="38"/>
+      <c r="B299">
+        <v>479</v>
+      </c>
       <c r="C299" s="3">
         <v>150</v>
       </c>
@@ -40601,18 +40605,20 @@
       </c>
       <c r="E299" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.2808219178082192</v>
       </c>
       <c r="F299" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.13670091324200914</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="51">
         <v>45964.999305497688</v>
       </c>
-      <c r="B300" s="38"/>
+      <c r="B300">
+        <v>312.60000000000002</v>
+      </c>
       <c r="C300" s="3">
         <v>150</v>
       </c>
@@ -40621,18 +40627,20 @@
       </c>
       <c r="E300" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2.1410958904109592</v>
       </c>
       <c r="F300" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>8.9212328767123289E-2</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="51">
         <v>45965.999305497688</v>
       </c>
-      <c r="B301" s="38"/>
+      <c r="B301">
+        <v>588.4</v>
+      </c>
       <c r="C301" s="3">
         <v>150</v>
       </c>
@@ -40641,18 +40649,20 @@
       </c>
       <c r="E301" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.0301369863013701</v>
       </c>
       <c r="F301" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.16792237442922373</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="51">
         <v>45966.999305497688</v>
       </c>
-      <c r="B302" s="38"/>
+      <c r="B302">
+        <v>670.5</v>
+      </c>
       <c r="C302" s="3">
         <v>150</v>
       </c>
@@ -40661,18 +40671,20 @@
       </c>
       <c r="E302" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.5924657534246576</v>
       </c>
       <c r="F302" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.1913527397260274</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="51">
         <v>45967.999305497688</v>
       </c>
-      <c r="B303" s="38"/>
+      <c r="B303">
+        <v>718.1</v>
+      </c>
       <c r="C303" s="3">
         <v>150</v>
       </c>
@@ -40681,18 +40693,20 @@
       </c>
       <c r="E303" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.9184931506849319</v>
       </c>
       <c r="F303" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.20493721461187214</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="51">
         <v>45968.999305497688</v>
       </c>
-      <c r="B304" s="38"/>
+      <c r="B304">
+        <v>586.6</v>
+      </c>
       <c r="C304" s="3">
         <v>150</v>
       </c>
@@ -40701,18 +40715,20 @@
       </c>
       <c r="E304" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.0178082191780824</v>
       </c>
       <c r="F304" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.16740867579908678</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="51">
         <v>45969.999305497688</v>
       </c>
-      <c r="B305" s="38"/>
+      <c r="B305">
+        <v>97.2</v>
+      </c>
       <c r="C305" s="3">
         <v>150</v>
       </c>
@@ -40721,18 +40737,20 @@
       </c>
       <c r="E305" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.66575342465753429</v>
       </c>
       <c r="F305" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2.7739726027397261E-2</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="51">
         <v>45970.999305497688</v>
       </c>
-      <c r="B306" s="38"/>
+      <c r="B306">
+        <v>322.2</v>
+      </c>
       <c r="C306" s="3">
         <v>150</v>
       </c>
@@ -40741,18 +40759,20 @@
       </c>
       <c r="E306" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2.2068493150684931</v>
       </c>
       <c r="F306" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>9.1952054794520538E-2</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="51">
         <v>45971.999305497688</v>
       </c>
-      <c r="B307" s="38"/>
+      <c r="B307">
+        <v>515.5</v>
+      </c>
       <c r="C307" s="3">
         <v>150</v>
       </c>
@@ -40761,18 +40781,20 @@
       </c>
       <c r="E307" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.5308219178082192</v>
       </c>
       <c r="F307" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.1471175799086758</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="51">
         <v>45972.999305497688</v>
       </c>
-      <c r="B308" s="38"/>
+      <c r="B308">
+        <v>698.2</v>
+      </c>
       <c r="C308" s="3">
         <v>150</v>
       </c>
@@ -40781,18 +40803,20 @@
       </c>
       <c r="E308" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.7821917808219183</v>
       </c>
       <c r="F308" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.19925799086757992</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="51">
         <v>45973.999305497688</v>
       </c>
-      <c r="B309" s="38"/>
+      <c r="B309">
+        <v>835.1</v>
+      </c>
       <c r="C309" s="3">
         <v>150</v>
       </c>
@@ -40801,18 +40825,20 @@
       </c>
       <c r="E309" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5.7198630136986299</v>
       </c>
       <c r="F309" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.23832762557077627</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="51">
         <v>45974.999305497688</v>
       </c>
-      <c r="B310" s="38"/>
+      <c r="B310">
+        <v>700.5</v>
+      </c>
       <c r="C310" s="3">
         <v>150</v>
       </c>
@@ -40821,18 +40847,20 @@
       </c>
       <c r="E310" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.7979452054794525</v>
       </c>
       <c r="F310" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.19991438356164384</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="51">
         <v>45975.999305497688</v>
       </c>
-      <c r="B311" s="38"/>
+      <c r="B311">
+        <v>685.7</v>
+      </c>
       <c r="C311" s="3">
         <v>150</v>
       </c>
@@ -40841,18 +40869,20 @@
       </c>
       <c r="E311" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.6965753424657537</v>
       </c>
       <c r="F311" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.19569063926940641</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="51">
         <v>45976.999305497688</v>
       </c>
-      <c r="B312" s="38"/>
+      <c r="B312">
+        <v>674.9</v>
+      </c>
       <c r="C312" s="3">
         <v>150</v>
       </c>
@@ -40861,18 +40891,20 @@
       </c>
       <c r="E312" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.6226027397260276</v>
       </c>
       <c r="F312" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.19260844748858447</v>
       </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="51">
         <v>45977.999305497688</v>
       </c>
-      <c r="B313" s="38"/>
+      <c r="B313">
+        <v>505</v>
+      </c>
       <c r="C313" s="3">
         <v>150</v>
       </c>
@@ -40881,18 +40913,20 @@
       </c>
       <c r="E313" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.4589041095890409</v>
       </c>
       <c r="F313" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.14412100456621005</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="51">
         <v>45978.999305497688</v>
       </c>
-      <c r="B314" s="38"/>
+      <c r="B314">
+        <v>239.8</v>
+      </c>
       <c r="C314" s="3">
         <v>150</v>
       </c>
@@ -40901,18 +40935,20 @@
       </c>
       <c r="E314" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1.6424657534246576</v>
       </c>
       <c r="F314" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>6.8436073059360739E-2</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="51">
         <v>45979.999305497688</v>
       </c>
-      <c r="B315" s="38"/>
+      <c r="B315">
+        <v>578.6</v>
+      </c>
       <c r="C315" s="3">
         <v>150</v>
       </c>
@@ -40921,18 +40957,20 @@
       </c>
       <c r="E315" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.963013698630137</v>
       </c>
       <c r="F315" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.16512557077625573</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="51">
         <v>45980.999305497688</v>
       </c>
-      <c r="B316" s="38"/>
+      <c r="B316">
+        <v>852</v>
+      </c>
       <c r="C316" s="3">
         <v>150</v>
       </c>
@@ -40941,18 +40979,20 @@
       </c>
       <c r="E316" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5.8356164383561646</v>
       </c>
       <c r="F316" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.24315068493150685</v>
       </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="51">
         <v>45981.999305497688</v>
       </c>
-      <c r="B317" s="38"/>
+      <c r="B317">
+        <v>838.8</v>
+      </c>
       <c r="C317" s="3">
         <v>150</v>
       </c>
@@ -40961,18 +41001,20 @@
       </c>
       <c r="E317" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5.7452054794520544</v>
       </c>
       <c r="F317" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.23938356164383559</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="51">
         <v>45982.999305497688</v>
       </c>
-      <c r="B318" s="38"/>
+      <c r="B318">
+        <v>765.4</v>
+      </c>
       <c r="C318" s="3">
         <v>150</v>
       </c>
@@ -40981,18 +41023,20 @@
       </c>
       <c r="E318" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5.242465753424657</v>
       </c>
       <c r="F318" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.21843607305936072</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="51">
         <v>45983.999305497688</v>
       </c>
-      <c r="B319" s="38"/>
+      <c r="B319">
+        <v>643.9</v>
+      </c>
       <c r="C319" s="3">
         <v>150</v>
       </c>
@@ -41001,18 +41045,20 @@
       </c>
       <c r="E319" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.4102739726027398</v>
       </c>
       <c r="F319" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.18376141552511416</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="51">
         <v>45984.999305497688</v>
       </c>
-      <c r="B320" s="38"/>
+      <c r="B320">
+        <v>196.1</v>
+      </c>
       <c r="C320" s="3">
         <v>150</v>
       </c>
@@ -41021,18 +41067,20 @@
       </c>
       <c r="E320" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1.3431506849315069</v>
       </c>
       <c r="F320" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>5.5964611872146117E-2</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="51">
         <v>45985.999305497688</v>
       </c>
-      <c r="B321" s="38"/>
+      <c r="B321">
+        <v>548.9</v>
+      </c>
       <c r="C321" s="3">
         <v>150</v>
       </c>
@@ -41041,18 +41089,20 @@
       </c>
       <c r="E321" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.7595890410958903</v>
       </c>
       <c r="F321" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.15664954337899542</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="51">
         <v>45986.999305497688</v>
       </c>
-      <c r="B322" s="38"/>
+      <c r="B322">
+        <v>552.6</v>
+      </c>
       <c r="C322" s="3">
         <v>150</v>
       </c>
@@ -41061,18 +41111,20 @@
       </c>
       <c r="E322" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3.7849315068493152</v>
       </c>
       <c r="F322" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.15770547945205479</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="51">
         <v>45987.999305497688</v>
       </c>
-      <c r="B323" s="38"/>
+      <c r="B323">
+        <v>727.9</v>
+      </c>
       <c r="C323" s="3">
         <v>150</v>
       </c>
@@ -41081,18 +41133,20 @@
       </c>
       <c r="E323" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.9856164383561641</v>
       </c>
       <c r="F323" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.20773401826484017</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="51">
         <v>45988.999305497688</v>
       </c>
-      <c r="B324" s="38"/>
+      <c r="B324">
+        <v>720.5</v>
+      </c>
       <c r="C324" s="3">
         <v>150</v>
       </c>
@@ -41101,18 +41155,20 @@
       </c>
       <c r="E324" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.9349315068493151</v>
       </c>
       <c r="F324" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.20562214611872145</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="51">
         <v>45989.999305497688</v>
       </c>
-      <c r="B325" s="38"/>
+      <c r="B325">
+        <v>707.6</v>
+      </c>
       <c r="C325" s="3">
         <v>150</v>
       </c>
@@ -41121,18 +41177,20 @@
       </c>
       <c r="E325" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.8465753424657532</v>
       </c>
       <c r="F325" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.20194063926940639</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="51">
         <v>45990.999305497688</v>
       </c>
-      <c r="B326" s="38"/>
+      <c r="B326">
+        <v>629.9</v>
+      </c>
       <c r="C326" s="3">
         <v>150</v>
       </c>
@@ -41141,18 +41199,20 @@
       </c>
       <c r="E326" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.3143835616438357</v>
       </c>
       <c r="F326" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.17976598173515981</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="51">
         <v>45991.999305497688</v>
       </c>
-      <c r="B327" s="38"/>
+      <c r="B327">
+        <v>710.8</v>
+      </c>
       <c r="C327" s="3">
         <v>150</v>
       </c>
@@ -41161,11 +41221,11 @@
       </c>
       <c r="E327" s="47">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4.8684931506849312</v>
       </c>
       <c r="F327" s="54">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.20285388127853879</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -41837,8 +41897,8 @@
   <sheetPr codeName="Planilha5"/>
   <dimension ref="A1:BW518"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H429" sqref="H429"/>
+    <sheetView topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43296,13 +43356,22 @@
         <f>AVERAGE(B427:B457)</f>
         <v>465.75806451612897</v>
       </c>
-      <c r="K31" s="65"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="28">
-        <f t="shared" ref="M31:M33" si="2">K31/(R31*30*D28)</f>
-        <v>0</v>
-      </c>
-      <c r="N31" s="28"/>
+      <c r="K31" s="65">
+        <f>SUM(B427:B457)/1000</f>
+        <v>14.438499999999998</v>
+      </c>
+      <c r="L31" s="20">
+        <f>SUM(E427:E457)</f>
+        <v>110.2175572519084</v>
+      </c>
+      <c r="M31" s="18">
+        <f>K31*1000/(R31*31*D28)</f>
+        <v>0.62816344039614935</v>
+      </c>
+      <c r="N31" s="18">
+        <f>AVERAGE(F427:F457)</f>
+        <v>0.1481418780267586</v>
+      </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="15" t="s">
         <v>16</v>
@@ -43335,14 +43404,26 @@
       <c r="I32" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="16"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="16"/>
+      <c r="J32" s="16">
+        <f>AVERAGE(B458:B487)</f>
+        <v>488.91</v>
+      </c>
+      <c r="K32" s="66">
+        <f>SUM(B458:B487)/1000</f>
+        <v>14.667300000000001</v>
+      </c>
+      <c r="L32" s="16">
+        <f>SUM(E458:E487)</f>
+        <v>111.9641221374046</v>
+      </c>
       <c r="M32" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="18"/>
+        <f>K32*1000/(R32*30*D29)</f>
+        <v>0.69759577655703797</v>
+      </c>
+      <c r="N32" s="18">
+        <f>AVERAGE(F458:F487)</f>
+        <v>0.15550572519083974</v>
+      </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="13" t="s">
         <v>17</v>
@@ -43378,11 +43459,14 @@
       <c r="J33" s="12"/>
       <c r="K33" s="65"/>
       <c r="L33" s="20"/>
-      <c r="M33" s="28">
-        <f t="shared" si="2"/>
+      <c r="M33" s="18">
+        <f>K33*1000/(R33*30*D30)</f>
         <v>0</v>
       </c>
-      <c r="N33" s="28"/>
+      <c r="N33" s="18">
+        <f t="shared" ref="N33" si="2">AVERAGE(F400:F429)</f>
+        <v>0.15613231552162843</v>
+      </c>
       <c r="P33" s="1"/>
       <c r="Q33" s="15" t="s">
         <v>18</v>
@@ -43417,23 +43501,23 @@
       </c>
       <c r="J34" s="33">
         <f>AVERAGE(J22:J33)</f>
-        <v>408.61131811414396</v>
+        <v>415.91119828558544</v>
       </c>
       <c r="K34" s="63">
         <f>SUM(K22:K33)</f>
-        <v>105.61069999999998</v>
+        <v>134.7165</v>
       </c>
       <c r="L34" s="33">
         <f>SUM(L22:L33)</f>
-        <v>808.75572519083971</v>
+        <v>1030.9374045801526</v>
       </c>
       <c r="M34" s="24">
         <f>K34*1000/(R34*365*131)</f>
-        <v>0.43055277824151267</v>
+        <v>0.54921104916426799</v>
       </c>
       <c r="N34" s="26">
         <f>AVERAGE(N22:N33)</f>
-        <v>0.1279458268527463</v>
+        <v>0.13427436336782864</v>
       </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="29" t="s">
@@ -43576,7 +43660,7 @@
       </c>
       <c r="M40" s="2">
         <f>AVERAGE(M22:M33)</f>
-        <v>0.45049640812469388</v>
+        <v>0.5609763428707929</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -51242,7 +51326,7 @@
         <v>3.4793893129770992</v>
       </c>
       <c r="F388" s="48">
-        <f t="shared" ref="F388:F448" si="16">B388/(24*D388)</f>
+        <f t="shared" ref="F388:F451" si="16">B388/(24*D388)</f>
         <v>0.14497455470737913</v>
       </c>
     </row>
@@ -52272,7 +52356,7 @@
         <v>131</v>
       </c>
       <c r="E435" s="56">
-        <f t="shared" ref="E435:E448" si="17">B435/D435</f>
+        <f t="shared" ref="E435:E498" si="17">B435/D435</f>
         <v>2.5465648854961835</v>
       </c>
       <c r="F435" s="48">
@@ -52573,10 +52657,20 @@
       <c r="B449">
         <v>434.9</v>
       </c>
-      <c r="C449" s="38"/>
-      <c r="D449" s="38"/>
-      <c r="E449" s="38"/>
-      <c r="F449" s="38"/>
+      <c r="C449" s="38">
+        <v>120</v>
+      </c>
+      <c r="D449" s="38">
+        <v>131</v>
+      </c>
+      <c r="E449" s="56">
+        <f t="shared" si="17"/>
+        <v>3.3198473282442746</v>
+      </c>
+      <c r="F449" s="48">
+        <f t="shared" si="16"/>
+        <v>0.1383269720101781</v>
+      </c>
     </row>
     <row r="450" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A450" s="51">
@@ -52585,10 +52679,20 @@
       <c r="B450">
         <v>455.8</v>
       </c>
-      <c r="C450" s="38"/>
-      <c r="D450" s="38"/>
-      <c r="E450" s="38"/>
-      <c r="F450" s="38"/>
+      <c r="C450" s="38">
+        <v>120</v>
+      </c>
+      <c r="D450" s="38">
+        <v>131</v>
+      </c>
+      <c r="E450" s="56">
+        <f t="shared" si="17"/>
+        <v>3.4793893129770992</v>
+      </c>
+      <c r="F450" s="48">
+        <f t="shared" si="16"/>
+        <v>0.14497455470737913</v>
+      </c>
     </row>
     <row r="451" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A451" s="51">
@@ -52597,10 +52701,20 @@
       <c r="B451">
         <v>600.9</v>
       </c>
-      <c r="C451" s="38"/>
-      <c r="D451" s="38"/>
-      <c r="E451" s="38"/>
-      <c r="F451" s="38"/>
+      <c r="C451" s="38">
+        <v>120</v>
+      </c>
+      <c r="D451" s="38">
+        <v>131</v>
+      </c>
+      <c r="E451" s="56">
+        <f t="shared" si="17"/>
+        <v>4.5870229007633583</v>
+      </c>
+      <c r="F451" s="48">
+        <f t="shared" si="16"/>
+        <v>0.19112595419847328</v>
+      </c>
     </row>
     <row r="452" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A452" s="51">
@@ -52609,10 +52723,20 @@
       <c r="B452">
         <v>557.70000000000005</v>
       </c>
-      <c r="C452" s="38"/>
-      <c r="D452" s="38"/>
-      <c r="E452" s="38"/>
-      <c r="F452" s="38"/>
+      <c r="C452" s="38">
+        <v>120</v>
+      </c>
+      <c r="D452" s="38">
+        <v>131</v>
+      </c>
+      <c r="E452" s="56">
+        <f t="shared" si="17"/>
+        <v>4.2572519083969471</v>
+      </c>
+      <c r="F452" s="48">
+        <f t="shared" ref="F452:F515" si="18">B452/(24*D452)</f>
+        <v>0.17738549618320612</v>
+      </c>
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A453" s="51">
@@ -52621,10 +52745,20 @@
       <c r="B453">
         <v>575</v>
       </c>
-      <c r="C453" s="38"/>
-      <c r="D453" s="38"/>
-      <c r="E453" s="38"/>
-      <c r="F453" s="38"/>
+      <c r="C453" s="38">
+        <v>120</v>
+      </c>
+      <c r="D453" s="38">
+        <v>131</v>
+      </c>
+      <c r="E453" s="56">
+        <f t="shared" si="17"/>
+        <v>4.3893129770992365</v>
+      </c>
+      <c r="F453" s="48">
+        <f t="shared" si="18"/>
+        <v>0.1828880407124682</v>
+      </c>
     </row>
     <row r="454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A454" s="51">
@@ -52633,10 +52767,20 @@
       <c r="B454">
         <v>525.29999999999995</v>
       </c>
-      <c r="C454" s="38"/>
-      <c r="D454" s="38"/>
-      <c r="E454" s="38"/>
-      <c r="F454" s="38"/>
+      <c r="C454" s="38">
+        <v>120</v>
+      </c>
+      <c r="D454" s="38">
+        <v>131</v>
+      </c>
+      <c r="E454" s="56">
+        <f t="shared" si="17"/>
+        <v>4.0099236641221374</v>
+      </c>
+      <c r="F454" s="48">
+        <f t="shared" si="18"/>
+        <v>0.16708015267175572</v>
+      </c>
     </row>
     <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455" s="51">
@@ -52645,10 +52789,20 @@
       <c r="B455">
         <v>487.3</v>
       </c>
-      <c r="C455" s="38"/>
-      <c r="D455" s="38"/>
-      <c r="E455" s="38"/>
-      <c r="F455" s="38"/>
+      <c r="C455" s="38">
+        <v>120</v>
+      </c>
+      <c r="D455" s="38">
+        <v>131</v>
+      </c>
+      <c r="E455" s="56">
+        <f t="shared" si="17"/>
+        <v>3.719847328244275</v>
+      </c>
+      <c r="F455" s="48">
+        <f t="shared" si="18"/>
+        <v>0.15499363867684479</v>
+      </c>
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A456" s="51">
@@ -52657,10 +52811,20 @@
       <c r="B456">
         <v>326.39999999999998</v>
       </c>
-      <c r="C456" s="38"/>
-      <c r="D456" s="38"/>
-      <c r="E456" s="38"/>
-      <c r="F456" s="38"/>
+      <c r="C456" s="38">
+        <v>120</v>
+      </c>
+      <c r="D456" s="38">
+        <v>131</v>
+      </c>
+      <c r="E456" s="56">
+        <f t="shared" si="17"/>
+        <v>2.4916030534351141</v>
+      </c>
+      <c r="F456" s="48">
+        <f t="shared" si="18"/>
+        <v>0.10381679389312977</v>
+      </c>
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A457" s="51">
@@ -52669,10 +52833,20 @@
       <c r="B457">
         <v>258.8</v>
       </c>
-      <c r="C457" s="38"/>
-      <c r="D457" s="38"/>
-      <c r="E457" s="38"/>
-      <c r="F457" s="38"/>
+      <c r="C457" s="38">
+        <v>120</v>
+      </c>
+      <c r="D457" s="38">
+        <v>131</v>
+      </c>
+      <c r="E457" s="56">
+        <f t="shared" si="17"/>
+        <v>1.9755725190839695</v>
+      </c>
+      <c r="F457" s="48">
+        <f t="shared" si="18"/>
+        <v>8.2315521628498728E-2</v>
+      </c>
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A458" s="51">
@@ -52681,10 +52855,20 @@
       <c r="B458">
         <v>552.9</v>
       </c>
-      <c r="C458" s="38"/>
-      <c r="D458" s="38"/>
-      <c r="E458" s="38"/>
-      <c r="F458" s="38"/>
+      <c r="C458" s="38">
+        <v>120</v>
+      </c>
+      <c r="D458" s="38">
+        <v>131</v>
+      </c>
+      <c r="E458" s="56">
+        <f t="shared" si="17"/>
+        <v>4.2206106870229005</v>
+      </c>
+      <c r="F458" s="48">
+        <f t="shared" si="18"/>
+        <v>0.1758587786259542</v>
+      </c>
     </row>
     <row r="459" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A459" s="51">
@@ -52693,10 +52877,20 @@
       <c r="B459">
         <v>390.6</v>
       </c>
-      <c r="C459" s="38"/>
-      <c r="D459" s="38"/>
-      <c r="E459" s="38"/>
-      <c r="F459" s="38"/>
+      <c r="C459" s="38">
+        <v>120</v>
+      </c>
+      <c r="D459" s="38">
+        <v>131</v>
+      </c>
+      <c r="E459" s="56">
+        <f t="shared" si="17"/>
+        <v>2.9816793893129772</v>
+      </c>
+      <c r="F459" s="48">
+        <f t="shared" si="18"/>
+        <v>0.12423664122137405</v>
+      </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A460" s="51">
@@ -52705,10 +52899,20 @@
       <c r="B460">
         <v>260.8</v>
       </c>
-      <c r="C460" s="38"/>
-      <c r="D460" s="38"/>
-      <c r="E460" s="38"/>
-      <c r="F460" s="38"/>
+      <c r="C460" s="38">
+        <v>120</v>
+      </c>
+      <c r="D460" s="38">
+        <v>131</v>
+      </c>
+      <c r="E460" s="56">
+        <f t="shared" si="17"/>
+        <v>1.9908396946564886</v>
+      </c>
+      <c r="F460" s="48">
+        <f t="shared" si="18"/>
+        <v>8.2951653944020362E-2</v>
+      </c>
     </row>
     <row r="461" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A461" s="51">
@@ -52717,10 +52921,20 @@
       <c r="B461">
         <v>488.4</v>
       </c>
-      <c r="C461" s="38"/>
-      <c r="D461" s="38"/>
-      <c r="E461" s="38"/>
-      <c r="F461" s="38"/>
+      <c r="C461" s="38">
+        <v>120</v>
+      </c>
+      <c r="D461" s="38">
+        <v>131</v>
+      </c>
+      <c r="E461" s="56">
+        <f t="shared" si="17"/>
+        <v>3.72824427480916</v>
+      </c>
+      <c r="F461" s="48">
+        <f t="shared" si="18"/>
+        <v>0.15534351145038167</v>
+      </c>
     </row>
     <row r="462" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A462" s="51">
@@ -52729,10 +52943,20 @@
       <c r="B462">
         <v>560.20000000000005</v>
       </c>
-      <c r="C462" s="38"/>
-      <c r="D462" s="38"/>
-      <c r="E462" s="38"/>
-      <c r="F462" s="38"/>
+      <c r="C462" s="38">
+        <v>120</v>
+      </c>
+      <c r="D462" s="38">
+        <v>131</v>
+      </c>
+      <c r="E462" s="56">
+        <f t="shared" si="17"/>
+        <v>4.2763358778625955</v>
+      </c>
+      <c r="F462" s="48">
+        <f t="shared" si="18"/>
+        <v>0.17818066157760815</v>
+      </c>
     </row>
     <row r="463" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A463" s="51">
@@ -52741,10 +52965,20 @@
       <c r="B463">
         <v>594.1</v>
       </c>
-      <c r="C463" s="38"/>
-      <c r="D463" s="38"/>
-      <c r="E463" s="38"/>
-      <c r="F463" s="38"/>
+      <c r="C463" s="38">
+        <v>120</v>
+      </c>
+      <c r="D463" s="38">
+        <v>131</v>
+      </c>
+      <c r="E463" s="56">
+        <f t="shared" si="17"/>
+        <v>4.5351145038167937</v>
+      </c>
+      <c r="F463" s="48">
+        <f t="shared" si="18"/>
+        <v>0.18896310432569977</v>
+      </c>
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A464" s="51">
@@ -52753,10 +52987,20 @@
       <c r="B464">
         <v>507.4</v>
       </c>
-      <c r="C464" s="38"/>
-      <c r="D464" s="38"/>
-      <c r="E464" s="38"/>
-      <c r="F464" s="38"/>
+      <c r="C464" s="38">
+        <v>120</v>
+      </c>
+      <c r="D464" s="38">
+        <v>131</v>
+      </c>
+      <c r="E464" s="56">
+        <f t="shared" si="17"/>
+        <v>3.8732824427480916</v>
+      </c>
+      <c r="F464" s="48">
+        <f t="shared" si="18"/>
+        <v>0.16138676844783714</v>
+      </c>
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A465" s="51">
@@ -52765,10 +53009,20 @@
       <c r="B465">
         <v>80.3</v>
       </c>
-      <c r="C465" s="38"/>
-      <c r="D465" s="38"/>
-      <c r="E465" s="38"/>
-      <c r="F465" s="38"/>
+      <c r="C465" s="38">
+        <v>120</v>
+      </c>
+      <c r="D465" s="38">
+        <v>131</v>
+      </c>
+      <c r="E465" s="56">
+        <f t="shared" si="17"/>
+        <v>0.61297709923664123</v>
+      </c>
+      <c r="F465" s="48">
+        <f t="shared" si="18"/>
+        <v>2.5540712468193384E-2</v>
+      </c>
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A466" s="51">
@@ -52777,10 +53031,20 @@
       <c r="B466">
         <v>273.60000000000002</v>
       </c>
-      <c r="C466" s="38"/>
-      <c r="D466" s="38"/>
-      <c r="E466" s="38"/>
-      <c r="F466" s="38"/>
+      <c r="C466" s="38">
+        <v>120</v>
+      </c>
+      <c r="D466" s="38">
+        <v>131</v>
+      </c>
+      <c r="E466" s="56">
+        <f t="shared" si="17"/>
+        <v>2.0885496183206107</v>
+      </c>
+      <c r="F466" s="48">
+        <f t="shared" si="18"/>
+        <v>8.7022900763358779E-2</v>
+      </c>
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A467" s="51">
@@ -52789,10 +53053,20 @@
       <c r="B467">
         <v>434.4</v>
       </c>
-      <c r="C467" s="38"/>
-      <c r="D467" s="38"/>
-      <c r="E467" s="38"/>
-      <c r="F467" s="38"/>
+      <c r="C467" s="38">
+        <v>120</v>
+      </c>
+      <c r="D467" s="38">
+        <v>131</v>
+      </c>
+      <c r="E467" s="56">
+        <f t="shared" si="17"/>
+        <v>3.3160305343511447</v>
+      </c>
+      <c r="F467" s="48">
+        <f t="shared" si="18"/>
+        <v>0.1381679389312977</v>
+      </c>
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A468" s="51">
@@ -52801,10 +53075,20 @@
       <c r="B468">
         <v>578.5</v>
       </c>
-      <c r="C468" s="38"/>
-      <c r="D468" s="38"/>
-      <c r="E468" s="38"/>
-      <c r="F468" s="38"/>
+      <c r="C468" s="38">
+        <v>120</v>
+      </c>
+      <c r="D468" s="38">
+        <v>131</v>
+      </c>
+      <c r="E468" s="56">
+        <f t="shared" si="17"/>
+        <v>4.4160305343511448</v>
+      </c>
+      <c r="F468" s="48">
+        <f t="shared" si="18"/>
+        <v>0.18400127226463103</v>
+      </c>
     </row>
     <row r="469" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A469" s="51">
@@ -52813,10 +53097,20 @@
       <c r="B469">
         <v>673.6</v>
       </c>
-      <c r="C469" s="38"/>
-      <c r="D469" s="38"/>
-      <c r="E469" s="38"/>
-      <c r="F469" s="38"/>
+      <c r="C469" s="38">
+        <v>120</v>
+      </c>
+      <c r="D469" s="38">
+        <v>131</v>
+      </c>
+      <c r="E469" s="56">
+        <f t="shared" si="17"/>
+        <v>5.1419847328244277</v>
+      </c>
+      <c r="F469" s="48">
+        <f t="shared" si="18"/>
+        <v>0.21424936386768448</v>
+      </c>
     </row>
     <row r="470" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A470" s="51">
@@ -52825,10 +53119,20 @@
       <c r="B470">
         <v>559.6</v>
       </c>
-      <c r="C470" s="38"/>
-      <c r="D470" s="38"/>
-      <c r="E470" s="38"/>
-      <c r="F470" s="38"/>
+      <c r="C470" s="38">
+        <v>120</v>
+      </c>
+      <c r="D470" s="38">
+        <v>131</v>
+      </c>
+      <c r="E470" s="56">
+        <f t="shared" si="17"/>
+        <v>4.2717557251908396</v>
+      </c>
+      <c r="F470" s="48">
+        <f t="shared" si="18"/>
+        <v>0.17798982188295165</v>
+      </c>
     </row>
     <row r="471" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A471" s="51">
@@ -52837,10 +53141,20 @@
       <c r="B471">
         <v>569</v>
       </c>
-      <c r="C471" s="38"/>
-      <c r="D471" s="38"/>
-      <c r="E471" s="38"/>
-      <c r="F471" s="38"/>
+      <c r="C471" s="38">
+        <v>120</v>
+      </c>
+      <c r="D471" s="38">
+        <v>131</v>
+      </c>
+      <c r="E471" s="56">
+        <f t="shared" si="17"/>
+        <v>4.343511450381679</v>
+      </c>
+      <c r="F471" s="48">
+        <f t="shared" si="18"/>
+        <v>0.18097964376590331</v>
+      </c>
     </row>
     <row r="472" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A472" s="51">
@@ -52849,10 +53163,20 @@
       <c r="B472">
         <v>541.20000000000005</v>
       </c>
-      <c r="C472" s="38"/>
-      <c r="D472" s="38"/>
-      <c r="E472" s="38"/>
-      <c r="F472" s="38"/>
+      <c r="C472" s="38">
+        <v>120</v>
+      </c>
+      <c r="D472" s="38">
+        <v>131</v>
+      </c>
+      <c r="E472" s="56">
+        <f t="shared" si="17"/>
+        <v>4.1312977099236647</v>
+      </c>
+      <c r="F472" s="48">
+        <f t="shared" si="18"/>
+        <v>0.1721374045801527</v>
+      </c>
     </row>
     <row r="473" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A473" s="51">
@@ -52861,10 +53185,20 @@
       <c r="B473">
         <v>408.6</v>
       </c>
-      <c r="C473" s="38"/>
-      <c r="D473" s="38"/>
-      <c r="E473" s="38"/>
-      <c r="F473" s="38"/>
+      <c r="C473" s="38">
+        <v>120</v>
+      </c>
+      <c r="D473" s="38">
+        <v>131</v>
+      </c>
+      <c r="E473" s="56">
+        <f t="shared" si="17"/>
+        <v>3.1190839694656489</v>
+      </c>
+      <c r="F473" s="48">
+        <f t="shared" si="18"/>
+        <v>0.12996183206106871</v>
+      </c>
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A474" s="51">
@@ -52873,450 +53207,926 @@
       <c r="B474">
         <v>200.7</v>
       </c>
-      <c r="C474" s="38"/>
-      <c r="D474" s="38"/>
-      <c r="E474" s="38"/>
-      <c r="F474" s="38"/>
+      <c r="C474" s="38">
+        <v>120</v>
+      </c>
+      <c r="D474" s="38">
+        <v>131</v>
+      </c>
+      <c r="E474" s="56">
+        <f t="shared" si="17"/>
+        <v>1.53206106870229</v>
+      </c>
+      <c r="F474" s="48">
+        <f t="shared" si="18"/>
+        <v>6.3835877862595411E-2</v>
+      </c>
     </row>
     <row r="475" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A475" s="51">
         <v>45979.999305497688</v>
       </c>
-      <c r="B475" s="38"/>
-      <c r="C475" s="38"/>
-      <c r="D475" s="38"/>
-      <c r="E475" s="38"/>
-      <c r="F475" s="38"/>
+      <c r="B475">
+        <v>474.4</v>
+      </c>
+      <c r="C475" s="38">
+        <v>120</v>
+      </c>
+      <c r="D475" s="38">
+        <v>131</v>
+      </c>
+      <c r="E475" s="56">
+        <f t="shared" si="17"/>
+        <v>3.6213740458015264</v>
+      </c>
+      <c r="F475" s="48">
+        <f t="shared" si="18"/>
+        <v>0.15089058524173027</v>
+      </c>
     </row>
     <row r="476" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A476" s="51">
         <v>45980.999305497688</v>
       </c>
-      <c r="B476" s="38"/>
-      <c r="C476" s="38"/>
-      <c r="D476" s="38"/>
-      <c r="E476" s="38"/>
-      <c r="F476" s="38"/>
+      <c r="B476">
+        <v>701.5</v>
+      </c>
+      <c r="C476" s="38">
+        <v>120</v>
+      </c>
+      <c r="D476" s="38">
+        <v>131</v>
+      </c>
+      <c r="E476" s="56">
+        <f t="shared" si="17"/>
+        <v>5.3549618320610683</v>
+      </c>
+      <c r="F476" s="48">
+        <f t="shared" si="18"/>
+        <v>0.22312340966921121</v>
+      </c>
     </row>
     <row r="477" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A477" s="51">
         <v>45981.999305497688</v>
       </c>
-      <c r="B477" s="38"/>
-      <c r="C477" s="38"/>
-      <c r="D477" s="38"/>
-      <c r="E477" s="38"/>
-      <c r="F477" s="38"/>
+      <c r="B477">
+        <v>697</v>
+      </c>
+      <c r="C477" s="38">
+        <v>120</v>
+      </c>
+      <c r="D477" s="38">
+        <v>131</v>
+      </c>
+      <c r="E477" s="56">
+        <f t="shared" si="17"/>
+        <v>5.3206106870229011</v>
+      </c>
+      <c r="F477" s="48">
+        <f t="shared" si="18"/>
+        <v>0.22169211195928754</v>
+      </c>
     </row>
     <row r="478" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A478" s="51">
         <v>45982.999305497688</v>
       </c>
-      <c r="B478" s="38"/>
-      <c r="C478" s="38"/>
-      <c r="D478" s="38"/>
-      <c r="E478" s="38"/>
-      <c r="F478" s="38"/>
+      <c r="B478">
+        <v>628.70000000000005</v>
+      </c>
+      <c r="C478" s="38">
+        <v>120</v>
+      </c>
+      <c r="D478" s="38">
+        <v>131</v>
+      </c>
+      <c r="E478" s="56">
+        <f t="shared" si="17"/>
+        <v>4.7992366412213743</v>
+      </c>
+      <c r="F478" s="48">
+        <f t="shared" si="18"/>
+        <v>0.19996819338422395</v>
+      </c>
     </row>
     <row r="479" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A479" s="51">
         <v>45983.999305497688</v>
       </c>
-      <c r="B479" s="38"/>
-      <c r="C479" s="38"/>
-      <c r="D479" s="38"/>
-      <c r="E479" s="38"/>
-      <c r="F479" s="38"/>
+      <c r="B479">
+        <v>535.70000000000005</v>
+      </c>
+      <c r="C479" s="38">
+        <v>120</v>
+      </c>
+      <c r="D479" s="38">
+        <v>131</v>
+      </c>
+      <c r="E479" s="56">
+        <f t="shared" si="17"/>
+        <v>4.0893129770992367</v>
+      </c>
+      <c r="F479" s="48">
+        <f t="shared" si="18"/>
+        <v>0.17038804071246821</v>
+      </c>
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A480" s="51">
         <v>45984.999305497688</v>
       </c>
-      <c r="B480" s="38"/>
-      <c r="C480" s="38"/>
-      <c r="D480" s="38"/>
-      <c r="E480" s="38"/>
-      <c r="F480" s="38"/>
+      <c r="B480">
+        <v>159.30000000000001</v>
+      </c>
+      <c r="C480" s="38">
+        <v>120</v>
+      </c>
+      <c r="D480" s="38">
+        <v>131</v>
+      </c>
+      <c r="E480" s="56">
+        <f t="shared" si="17"/>
+        <v>1.2160305343511451</v>
+      </c>
+      <c r="F480" s="48">
+        <f t="shared" si="18"/>
+        <v>5.0667938931297715E-2</v>
+      </c>
     </row>
     <row r="481" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A481" s="51">
         <v>45985.999305497688</v>
       </c>
-      <c r="B481" s="38"/>
-      <c r="C481" s="38"/>
-      <c r="D481" s="38"/>
-      <c r="E481" s="38"/>
-      <c r="F481" s="38"/>
+      <c r="B481">
+        <v>450.7</v>
+      </c>
+      <c r="C481" s="38">
+        <v>120</v>
+      </c>
+      <c r="D481" s="38">
+        <v>131</v>
+      </c>
+      <c r="E481" s="56">
+        <f t="shared" si="17"/>
+        <v>3.4404580152671755</v>
+      </c>
+      <c r="F481" s="48">
+        <f t="shared" si="18"/>
+        <v>0.14335241730279899</v>
+      </c>
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A482" s="51">
         <v>45986.999305497688</v>
       </c>
-      <c r="B482" s="38"/>
-      <c r="C482" s="38"/>
-      <c r="D482" s="38"/>
-      <c r="E482" s="38"/>
-      <c r="F482" s="38"/>
+      <c r="B482">
+        <v>487.5</v>
+      </c>
+      <c r="C482" s="38">
+        <v>120</v>
+      </c>
+      <c r="D482" s="38">
+        <v>131</v>
+      </c>
+      <c r="E482" s="56">
+        <f t="shared" si="17"/>
+        <v>3.7213740458015265</v>
+      </c>
+      <c r="F482" s="48">
+        <f t="shared" si="18"/>
+        <v>0.15505725190839695</v>
+      </c>
     </row>
     <row r="483" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A483" s="51">
         <v>45987.999305497688</v>
       </c>
-      <c r="B483" s="38"/>
-      <c r="C483" s="38"/>
-      <c r="D483" s="38"/>
-      <c r="E483" s="38"/>
-      <c r="F483" s="38"/>
+      <c r="B483">
+        <v>617.9</v>
+      </c>
+      <c r="C483" s="38">
+        <v>120</v>
+      </c>
+      <c r="D483" s="38">
+        <v>131</v>
+      </c>
+      <c r="E483" s="56">
+        <f t="shared" si="17"/>
+        <v>4.716793893129771</v>
+      </c>
+      <c r="F483" s="48">
+        <f t="shared" si="18"/>
+        <v>0.19653307888040711</v>
+      </c>
     </row>
     <row r="484" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A484" s="51">
         <v>45988.999305497688</v>
       </c>
-      <c r="B484" s="38"/>
-      <c r="C484" s="38"/>
-      <c r="D484" s="38"/>
-      <c r="E484" s="38"/>
-      <c r="F484" s="38"/>
+      <c r="B484">
+        <v>572.1</v>
+      </c>
+      <c r="C484" s="38">
+        <v>120</v>
+      </c>
+      <c r="D484" s="38">
+        <v>131</v>
+      </c>
+      <c r="E484" s="56">
+        <f t="shared" si="17"/>
+        <v>4.3671755725190842</v>
+      </c>
+      <c r="F484" s="48">
+        <f t="shared" si="18"/>
+        <v>0.18196564885496183</v>
+      </c>
     </row>
     <row r="485" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A485" s="51">
         <v>45989.999305497688</v>
       </c>
-      <c r="B485" s="38"/>
-      <c r="C485" s="38"/>
-      <c r="D485" s="38"/>
-      <c r="E485" s="38"/>
-      <c r="F485" s="38"/>
+      <c r="B485">
+        <v>567.1</v>
+      </c>
+      <c r="C485" s="38">
+        <v>120</v>
+      </c>
+      <c r="D485" s="38">
+        <v>131</v>
+      </c>
+      <c r="E485" s="56">
+        <f t="shared" si="17"/>
+        <v>4.3290076335877865</v>
+      </c>
+      <c r="F485" s="48">
+        <f t="shared" si="18"/>
+        <v>0.18037531806615778</v>
+      </c>
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A486" s="51">
         <v>45990.999305497688</v>
       </c>
-      <c r="B486" s="38"/>
-      <c r="C486" s="38"/>
-      <c r="D486" s="38"/>
-      <c r="E486" s="38"/>
-      <c r="F486" s="38"/>
+      <c r="B486">
+        <v>525.79999999999995</v>
+      </c>
+      <c r="C486" s="38">
+        <v>120</v>
+      </c>
+      <c r="D486" s="38">
+        <v>131</v>
+      </c>
+      <c r="E486" s="56">
+        <f t="shared" si="17"/>
+        <v>4.0137404580152669</v>
+      </c>
+      <c r="F486" s="48">
+        <f t="shared" si="18"/>
+        <v>0.16723918575063612</v>
+      </c>
     </row>
     <row r="487" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A487" s="51">
         <v>45991.999305497688</v>
       </c>
-      <c r="B487" s="38"/>
-      <c r="C487" s="38"/>
-      <c r="D487" s="38"/>
-      <c r="E487" s="38"/>
-      <c r="F487" s="38"/>
+      <c r="B487">
+        <v>575.70000000000005</v>
+      </c>
+      <c r="C487" s="38">
+        <v>120</v>
+      </c>
+      <c r="D487" s="38">
+        <v>131</v>
+      </c>
+      <c r="E487" s="56">
+        <f t="shared" si="17"/>
+        <v>4.3946564885496189</v>
+      </c>
+      <c r="F487" s="48">
+        <f t="shared" si="18"/>
+        <v>0.18311068702290079</v>
+      </c>
     </row>
     <row r="488" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A488" s="51">
         <v>45992.999305497688</v>
       </c>
       <c r="B488" s="38"/>
-      <c r="C488" s="38"/>
-      <c r="D488" s="38"/>
-      <c r="E488" s="38"/>
-      <c r="F488" s="38"/>
+      <c r="C488" s="38">
+        <v>120</v>
+      </c>
+      <c r="D488" s="38">
+        <v>131</v>
+      </c>
+      <c r="E488" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F488" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="489" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A489" s="51">
         <v>45993.999305497688</v>
       </c>
       <c r="B489" s="38"/>
-      <c r="C489" s="38"/>
-      <c r="D489" s="38"/>
-      <c r="E489" s="38"/>
-      <c r="F489" s="38"/>
+      <c r="C489" s="38">
+        <v>120</v>
+      </c>
+      <c r="D489" s="38">
+        <v>131</v>
+      </c>
+      <c r="E489" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F489" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="490" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A490" s="51">
         <v>45994.999305497688</v>
       </c>
       <c r="B490" s="38"/>
-      <c r="C490" s="38"/>
-      <c r="D490" s="38"/>
-      <c r="E490" s="38"/>
-      <c r="F490" s="38"/>
+      <c r="C490" s="38">
+        <v>120</v>
+      </c>
+      <c r="D490" s="38">
+        <v>131</v>
+      </c>
+      <c r="E490" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F490" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="491" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A491" s="51">
         <v>45995.999305497688</v>
       </c>
       <c r="B491" s="38"/>
-      <c r="C491" s="38"/>
-      <c r="D491" s="38"/>
-      <c r="E491" s="38"/>
-      <c r="F491" s="38"/>
+      <c r="C491" s="38">
+        <v>120</v>
+      </c>
+      <c r="D491" s="38">
+        <v>131</v>
+      </c>
+      <c r="E491" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F491" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="492" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A492" s="51">
         <v>45996.999305497688</v>
       </c>
       <c r="B492" s="38"/>
-      <c r="C492" s="38"/>
-      <c r="D492" s="38"/>
-      <c r="E492" s="38"/>
-      <c r="F492" s="38"/>
+      <c r="C492" s="38">
+        <v>120</v>
+      </c>
+      <c r="D492" s="38">
+        <v>131</v>
+      </c>
+      <c r="E492" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F492" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="493" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A493" s="51">
         <v>45997.999305497688</v>
       </c>
       <c r="B493" s="38"/>
-      <c r="C493" s="38"/>
-      <c r="D493" s="38"/>
-      <c r="E493" s="38"/>
-      <c r="F493" s="38"/>
+      <c r="C493" s="38">
+        <v>120</v>
+      </c>
+      <c r="D493" s="38">
+        <v>131</v>
+      </c>
+      <c r="E493" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F493" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="494" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A494" s="51">
         <v>45998.999305497688</v>
       </c>
       <c r="B494" s="38"/>
-      <c r="C494" s="38"/>
-      <c r="D494" s="38"/>
-      <c r="E494" s="38"/>
-      <c r="F494" s="38"/>
+      <c r="C494" s="38">
+        <v>120</v>
+      </c>
+      <c r="D494" s="38">
+        <v>131</v>
+      </c>
+      <c r="E494" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F494" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="495" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A495" s="51">
         <v>45999.999305497688</v>
       </c>
       <c r="B495" s="38"/>
-      <c r="C495" s="38"/>
-      <c r="D495" s="38"/>
-      <c r="E495" s="38"/>
-      <c r="F495" s="38"/>
+      <c r="C495" s="38">
+        <v>120</v>
+      </c>
+      <c r="D495" s="38">
+        <v>131</v>
+      </c>
+      <c r="E495" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F495" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="496" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A496" s="51">
         <v>46000.999305497688</v>
       </c>
       <c r="B496" s="38"/>
-      <c r="C496" s="38"/>
-      <c r="D496" s="38"/>
-      <c r="E496" s="38"/>
-      <c r="F496" s="38"/>
+      <c r="C496" s="38">
+        <v>120</v>
+      </c>
+      <c r="D496" s="38">
+        <v>131</v>
+      </c>
+      <c r="E496" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F496" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="497" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A497" s="51">
         <v>46001.999305497688</v>
       </c>
       <c r="B497" s="38"/>
-      <c r="C497" s="38"/>
-      <c r="D497" s="38"/>
-      <c r="E497" s="38"/>
-      <c r="F497" s="38"/>
+      <c r="C497" s="38">
+        <v>120</v>
+      </c>
+      <c r="D497" s="38">
+        <v>131</v>
+      </c>
+      <c r="E497" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F497" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="498" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A498" s="51">
         <v>46002.999305497688</v>
       </c>
       <c r="B498" s="38"/>
-      <c r="C498" s="38"/>
-      <c r="D498" s="38"/>
-      <c r="E498" s="38"/>
-      <c r="F498" s="38"/>
+      <c r="C498" s="38">
+        <v>120</v>
+      </c>
+      <c r="D498" s="38">
+        <v>131</v>
+      </c>
+      <c r="E498" s="56">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F498" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="499" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A499" s="51">
         <v>46003.999305497688</v>
       </c>
       <c r="B499" s="38"/>
-      <c r="C499" s="38"/>
-      <c r="D499" s="38"/>
-      <c r="E499" s="38"/>
-      <c r="F499" s="38"/>
+      <c r="C499" s="38">
+        <v>120</v>
+      </c>
+      <c r="D499" s="38">
+        <v>131</v>
+      </c>
+      <c r="E499" s="56">
+        <f t="shared" ref="E499:E518" si="19">B499/D499</f>
+        <v>0</v>
+      </c>
+      <c r="F499" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A500" s="51">
         <v>46004.999305497688</v>
       </c>
       <c r="B500" s="38"/>
-      <c r="C500" s="38"/>
-      <c r="D500" s="38"/>
-      <c r="E500" s="38"/>
-      <c r="F500" s="38"/>
+      <c r="C500" s="38">
+        <v>120</v>
+      </c>
+      <c r="D500" s="38">
+        <v>131</v>
+      </c>
+      <c r="E500" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F500" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A501" s="51">
         <v>46005.999305497688</v>
       </c>
       <c r="B501" s="38"/>
-      <c r="C501" s="38"/>
-      <c r="D501" s="38"/>
-      <c r="E501" s="38"/>
-      <c r="F501" s="38"/>
+      <c r="C501" s="38">
+        <v>120</v>
+      </c>
+      <c r="D501" s="38">
+        <v>131</v>
+      </c>
+      <c r="E501" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F501" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="502" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A502" s="51">
         <v>46006.999305497688</v>
       </c>
       <c r="B502" s="38"/>
-      <c r="C502" s="38"/>
-      <c r="D502" s="38"/>
-      <c r="E502" s="38"/>
-      <c r="F502" s="38"/>
+      <c r="C502" s="38">
+        <v>120</v>
+      </c>
+      <c r="D502" s="38">
+        <v>131</v>
+      </c>
+      <c r="E502" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F502" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="503" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A503" s="51">
         <v>46007.999305497688</v>
       </c>
       <c r="B503" s="38"/>
-      <c r="C503" s="38"/>
-      <c r="D503" s="38"/>
-      <c r="E503" s="38"/>
-      <c r="F503" s="38"/>
+      <c r="C503" s="38">
+        <v>120</v>
+      </c>
+      <c r="D503" s="38">
+        <v>131</v>
+      </c>
+      <c r="E503" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F503" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="504" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A504" s="51">
         <v>46008.999305497688</v>
       </c>
       <c r="B504" s="38"/>
-      <c r="C504" s="38"/>
-      <c r="D504" s="38"/>
-      <c r="E504" s="38"/>
-      <c r="F504" s="38"/>
+      <c r="C504" s="38">
+        <v>120</v>
+      </c>
+      <c r="D504" s="38">
+        <v>131</v>
+      </c>
+      <c r="E504" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F504" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="505" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A505" s="51">
         <v>46009.999305497688</v>
       </c>
       <c r="B505" s="38"/>
-      <c r="C505" s="38"/>
-      <c r="D505" s="38"/>
-      <c r="E505" s="38"/>
-      <c r="F505" s="38"/>
+      <c r="C505" s="38">
+        <v>120</v>
+      </c>
+      <c r="D505" s="38">
+        <v>131</v>
+      </c>
+      <c r="E505" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F505" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="506" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A506" s="51">
         <v>46010.999305497688</v>
       </c>
       <c r="B506" s="38"/>
-      <c r="C506" s="38"/>
-      <c r="D506" s="38"/>
-      <c r="E506" s="38"/>
-      <c r="F506" s="38"/>
+      <c r="C506" s="38">
+        <v>120</v>
+      </c>
+      <c r="D506" s="38">
+        <v>131</v>
+      </c>
+      <c r="E506" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F506" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="507" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A507" s="51">
         <v>46011.999305497688</v>
       </c>
       <c r="B507" s="38"/>
-      <c r="C507" s="38"/>
-      <c r="D507" s="38"/>
-      <c r="E507" s="38"/>
-      <c r="F507" s="38"/>
+      <c r="C507" s="38">
+        <v>120</v>
+      </c>
+      <c r="D507" s="38">
+        <v>131</v>
+      </c>
+      <c r="E507" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F507" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="508" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A508" s="51">
         <v>46012.999305497688</v>
       </c>
       <c r="B508" s="38"/>
-      <c r="C508" s="38"/>
-      <c r="D508" s="38"/>
-      <c r="E508" s="38"/>
-      <c r="F508" s="38"/>
+      <c r="C508" s="38">
+        <v>120</v>
+      </c>
+      <c r="D508" s="38">
+        <v>131</v>
+      </c>
+      <c r="E508" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F508" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="509" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A509" s="51">
         <v>46013.999305497688</v>
       </c>
       <c r="B509" s="38"/>
-      <c r="C509" s="38"/>
-      <c r="D509" s="38"/>
-      <c r="E509" s="38"/>
-      <c r="F509" s="38"/>
+      <c r="C509" s="38">
+        <v>120</v>
+      </c>
+      <c r="D509" s="38">
+        <v>131</v>
+      </c>
+      <c r="E509" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F509" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A510" s="51">
         <v>46014.999305497688</v>
       </c>
       <c r="B510" s="38"/>
-      <c r="C510" s="38"/>
-      <c r="D510" s="38"/>
-      <c r="E510" s="38"/>
-      <c r="F510" s="38"/>
+      <c r="C510" s="38">
+        <v>120</v>
+      </c>
+      <c r="D510" s="38">
+        <v>131</v>
+      </c>
+      <c r="E510" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F510" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A511" s="51">
         <v>46015.999305497688</v>
       </c>
       <c r="B511" s="38"/>
-      <c r="C511" s="38"/>
-      <c r="D511" s="38"/>
-      <c r="E511" s="38"/>
-      <c r="F511" s="38"/>
+      <c r="C511" s="38">
+        <v>120</v>
+      </c>
+      <c r="D511" s="38">
+        <v>131</v>
+      </c>
+      <c r="E511" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F511" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A512" s="51">
         <v>46016.999305497688</v>
       </c>
       <c r="B512" s="38"/>
-      <c r="C512" s="38"/>
-      <c r="D512" s="38"/>
-      <c r="E512" s="38"/>
-      <c r="F512" s="38"/>
+      <c r="C512" s="38">
+        <v>120</v>
+      </c>
+      <c r="D512" s="38">
+        <v>131</v>
+      </c>
+      <c r="E512" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F512" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="513" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A513" s="51">
         <v>46017.999305497688</v>
       </c>
       <c r="B513" s="38"/>
-      <c r="C513" s="38"/>
-      <c r="D513" s="38"/>
-      <c r="E513" s="38"/>
-      <c r="F513" s="38"/>
+      <c r="C513" s="38">
+        <v>120</v>
+      </c>
+      <c r="D513" s="38">
+        <v>131</v>
+      </c>
+      <c r="E513" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F513" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="514" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A514" s="51">
         <v>46018.999305497688</v>
       </c>
       <c r="B514" s="38"/>
-      <c r="C514" s="38"/>
-      <c r="D514" s="38"/>
-      <c r="E514" s="38"/>
-      <c r="F514" s="38"/>
+      <c r="C514" s="38">
+        <v>120</v>
+      </c>
+      <c r="D514" s="38">
+        <v>131</v>
+      </c>
+      <c r="E514" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F514" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="515" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A515" s="51">
         <v>46019.999305497688</v>
       </c>
       <c r="B515" s="38"/>
-      <c r="C515" s="38"/>
-      <c r="D515" s="38"/>
-      <c r="E515" s="38"/>
-      <c r="F515" s="38"/>
+      <c r="C515" s="38">
+        <v>120</v>
+      </c>
+      <c r="D515" s="38">
+        <v>131</v>
+      </c>
+      <c r="E515" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F515" s="48">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="516" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A516" s="51">
         <v>46020.999305497688</v>
       </c>
       <c r="B516" s="38"/>
-      <c r="C516" s="38"/>
-      <c r="D516" s="38"/>
-      <c r="E516" s="38"/>
-      <c r="F516" s="38"/>
+      <c r="C516" s="38">
+        <v>120</v>
+      </c>
+      <c r="D516" s="38">
+        <v>131</v>
+      </c>
+      <c r="E516" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F516" s="48">
+        <f t="shared" ref="F516:F518" si="20">B516/(24*D516)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="517" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A517" s="51">
         <v>46021.999305497688</v>
       </c>
       <c r="B517" s="38"/>
-      <c r="C517" s="38"/>
-      <c r="D517" s="38"/>
-      <c r="E517" s="38"/>
-      <c r="F517" s="38"/>
+      <c r="C517" s="38">
+        <v>120</v>
+      </c>
+      <c r="D517" s="38">
+        <v>131</v>
+      </c>
+      <c r="E517" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F517" s="48">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="518" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A518" s="51">
         <v>46022.999305497688</v>
       </c>
       <c r="B518" s="38"/>
-      <c r="C518" s="38"/>
-      <c r="D518" s="38"/>
-      <c r="E518" s="38"/>
-      <c r="F518" s="38"/>
+      <c r="C518" s="38">
+        <v>120</v>
+      </c>
+      <c r="D518" s="38">
+        <v>131</v>
+      </c>
+      <c r="E518" s="56">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F518" s="48">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -60463,11 +61273,7 @@
       <c r="A5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75">
+      <c r="H5">
         <v>451</v>
       </c>
     </row>
@@ -60475,11 +61281,7 @@
       <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75">
+      <c r="H6">
         <v>119</v>
       </c>
     </row>
@@ -60487,11 +61289,7 @@
       <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75">
+      <c r="H7">
         <v>59</v>
       </c>
     </row>
@@ -60499,11 +61297,7 @@
       <c r="A8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75">
+      <c r="H8">
         <v>8</v>
       </c>
     </row>
@@ -60511,63 +61305,45 @@
       <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75">
+      <c r="F9">
         <v>2</v>
       </c>
-      <c r="G9" s="75">
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="H9" s="75"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="75">
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75">
+      <c r="E12">
         <v>4</v>
       </c>
-      <c r="F12" s="75">
+      <c r="F12">
         <v>1</v>
       </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75">
+      <c r="H13">
         <v>10</v>
       </c>
     </row>
@@ -60575,11 +61351,7 @@
       <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75">
+      <c r="H14">
         <v>19</v>
       </c>
     </row>
@@ -60587,11 +61359,7 @@
       <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75">
+      <c r="H15">
         <v>58</v>
       </c>
     </row>
@@ -60599,11 +61367,7 @@
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75">
+      <c r="H16">
         <v>133</v>
       </c>
     </row>

</xml_diff>